<commit_message>
Created FrameWork and Added TestCases for REPORT Module
</commit_message>
<xml_diff>
--- a/ActiTime/testdata/data.xlsx
+++ b/ActiTime/testdata/data.xlsx
@@ -2,16 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sandhya's Folder\workspace\ActiTimeApp\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="5145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="TC001" sheetId="1" r:id="rId1"/>
-    <sheet name="TC002" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:M15"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,30 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>username</t>
+    <t>ChartName</t>
   </si>
   <si>
-    <t>password</t>
+    <t>praba</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>manager</t>
-  </si>
-  <si>
-    <t>avc123</t>
-  </si>
-  <si>
-    <t>mohan</t>
+    <t>Timing Chart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,9 +133,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -174,9 +168,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -356,62 +350,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>